<commit_message>
feat: maintenance state added
</commit_message>
<xml_diff>
--- a/overview.xlsx
+++ b/overview.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rjp\Desktop\MocaGithub\13. stakingPro\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C05B0DE-F752-402E-B101-53246CF8BE2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69A0BD31-81E5-4DFA-8C92-E7A6AD29E382}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{C11E81BD-8086-48B4-8DA7-632AA4FADE65}"/>
   </bookViews>
@@ -16,6 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="50">
   <si>
     <t>Fn</t>
   </si>
@@ -144,12 +145,6 @@
     <t>only callable by RP contract</t>
   </si>
   <si>
-    <t>pack library return variables into struct</t>
-  </si>
-  <si>
-    <t>can use uint128</t>
-  </si>
-  <si>
     <t>callable by us; but does not need accessControl</t>
   </si>
   <si>
@@ -166,6 +161,30 @@
   </si>
   <si>
     <t>whenNotFrozen</t>
+  </si>
+  <si>
+    <t>owner</t>
+  </si>
+  <si>
+    <t>operator</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> pause</t>
+  </si>
+  <si>
+    <t>callable after ended</t>
+  </si>
+  <si>
+    <t>reset operator to 0 addr after each update</t>
+  </si>
+  <si>
+    <t>operater can reset, owner can reset</t>
+  </si>
+  <si>
+    <t>but only owner can set to new</t>
+  </si>
+  <si>
+    <t>if frozen, was paused</t>
   </si>
 </sst>
 </file>
@@ -213,7 +232,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -243,8 +262,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -289,12 +314,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -321,6 +355,13 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -636,10 +677,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D544DF9-B6D7-473E-A453-2471533C1400}">
-  <dimension ref="A1:O32"/>
+  <dimension ref="A1:R41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R25" sqref="R25"/>
+      <selection activeCell="T10" sqref="T10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -649,7 +690,7 @@
     <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="26.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16" customWidth="1"/>
+    <col min="6" max="6" width="20.42578125" customWidth="1"/>
     <col min="7" max="7" width="21" customWidth="1"/>
   </cols>
   <sheetData>
@@ -661,7 +702,7 @@
         <v>3</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
@@ -670,7 +711,7 @@
         <v>2</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>4</v>
@@ -680,6 +721,11 @@
       <c r="A2" s="5" t="s">
         <v>5</v>
       </c>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="16" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
@@ -687,7 +733,7 @@
       </c>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
+      <c r="F3" s="16"/>
       <c r="G3" t="s">
         <v>34</v>
       </c>
@@ -698,7 +744,7 @@
       </c>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
+      <c r="F4" s="16"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
@@ -706,7 +752,7 @@
       </c>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
+      <c r="F5" s="16"/>
       <c r="G5" t="s">
         <v>35</v>
       </c>
@@ -716,8 +762,11 @@
         <v>10</v>
       </c>
       <c r="B6" s="3"/>
+      <c r="D6" t="s">
+        <v>45</v>
+      </c>
       <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
+      <c r="F6" s="16"/>
       <c r="N6" s="5"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
@@ -726,15 +775,18 @@
       </c>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
+      <c r="F7" s="16"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>11</v>
       </c>
       <c r="B8" s="3"/>
+      <c r="D8" t="s">
+        <v>45</v>
+      </c>
       <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
+      <c r="F8" s="16"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
@@ -742,7 +794,7 @@
       </c>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
+      <c r="F9" s="16"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
@@ -750,7 +802,7 @@
       </c>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
+      <c r="F10" s="16"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
@@ -758,9 +810,9 @@
       </c>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
+      <c r="F11" s="16"/>
       <c r="G11" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
@@ -771,7 +823,7 @@
         <v>3</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>1</v>
@@ -780,13 +832,10 @@
         <v>2</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="G13" s="2" t="s">
         <v>4</v>
-      </c>
-      <c r="N13" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
@@ -797,9 +846,6 @@
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
       <c r="G14" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="N14" t="s">
         <v>37</v>
       </c>
     </row>
@@ -810,7 +856,7 @@
       <c r="C15" s="3"/>
       <c r="F15" s="3"/>
       <c r="G15" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
@@ -820,52 +866,52 @@
       <c r="C16" s="3"/>
       <c r="F16" s="3"/>
       <c r="G16" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>27</v>
       </c>
       <c r="C17" s="3"/>
       <c r="F17" s="3"/>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>21</v>
       </c>
       <c r="C18" s="3"/>
       <c r="F18" s="3"/>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>22</v>
       </c>
       <c r="C19" s="3"/>
       <c r="F19" s="3"/>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
         <v>23</v>
       </c>
       <c r="C20" s="3"/>
       <c r="F20" s="3"/>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
         <v>24</v>
       </c>
       <c r="C21" s="3"/>
       <c r="F21" s="3"/>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="s">
         <v>25</v>
       </c>
       <c r="C22" s="3"/>
       <c r="F22" s="3"/>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
         <v>17</v>
       </c>
@@ -873,28 +919,28 @@
       <c r="E23" s="3"/>
       <c r="F23" s="3"/>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
         <v>18</v>
       </c>
       <c r="C24" s="3"/>
       <c r="F24" s="3"/>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
         <v>19</v>
       </c>
       <c r="C25" s="3"/>
       <c r="F25" s="3"/>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26" s="8" t="s">
         <v>20</v>
       </c>
       <c r="C26" s="3"/>
       <c r="F26" s="3"/>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A28" s="9" t="s">
         <v>0</v>
       </c>
@@ -913,26 +959,100 @@
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
         <v>28</v>
       </c>
       <c r="O29" s="11"/>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="L30" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="M30" s="12" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="L31" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="M31" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="R31" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
         <v>31</v>
       </c>
+      <c r="L32" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="M32" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="R32" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="33" spans="12:18" x14ac:dyDescent="0.25">
+      <c r="L33" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="M33" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="R33" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="34" spans="12:18" x14ac:dyDescent="0.25">
+      <c r="L34" s="13"/>
+      <c r="M34" s="8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="35" spans="12:18" x14ac:dyDescent="0.25">
+      <c r="L35" s="13"/>
+      <c r="M35" s="14" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="36" spans="12:18" x14ac:dyDescent="0.25">
+      <c r="L36" s="13"/>
+      <c r="M36" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="37" spans="12:18" x14ac:dyDescent="0.25">
+      <c r="L37" s="13"/>
+      <c r="M37" s="7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="38" spans="12:18" x14ac:dyDescent="0.25">
+      <c r="L38" s="13"/>
+      <c r="M38" s="8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="39" spans="12:18" x14ac:dyDescent="0.25">
+      <c r="L39" s="13"/>
+    </row>
+    <row r="40" spans="12:18" x14ac:dyDescent="0.25">
+      <c r="L40" s="13"/>
+    </row>
+    <row r="41" spans="12:18" x14ac:dyDescent="0.25">
+      <c r="L41" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>